<commit_message>
Modificaciones para página WEB
</commit_message>
<xml_diff>
--- a/Opioides_RAM.xlsx
+++ b/Opioides_RAM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\Reacciones_Morfina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\Estudio_Documentos\Estadistica_2013-2\Regresion\007_Modelos_GLM\Binominal\Reacciones_Morfina\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Meperidina" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="S11" sheetId="9" r:id="rId7"/>
     <sheet name="S12" sheetId="12" r:id="rId8"/>
     <sheet name="RAM" sheetId="8" r:id="rId9"/>
+    <sheet name="S20" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="53">
   <si>
     <t>Preoperative</t>
   </si>
@@ -182,6 +183,15 @@
   </si>
   <si>
     <t>Mareo</t>
+  </si>
+  <si>
+    <t>Marcada</t>
+  </si>
+  <si>
+    <t>Moderada</t>
+  </si>
+  <si>
+    <t>Leve</t>
   </si>
 </sst>
 </file>
@@ -2766,7 +2776,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:P2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3565,6 +3575,433 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="15" width="4.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19">
+        <v>11</v>
+      </c>
+      <c r="D5" s="19">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="19">
+        <v>8</v>
+      </c>
+      <c r="D6" s="19">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>29</v>
+      </c>
+      <c r="D7" s="19">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="C8" s="19">
+        <v>33</v>
+      </c>
+      <c r="D8" s="19">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="19">
+        <v>1.8</v>
+      </c>
+      <c r="C9" s="19">
+        <v>32</v>
+      </c>
+      <c r="D9" s="19">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="19">
+        <v>2</v>
+      </c>
+      <c r="C10" s="19">
+        <v>33</v>
+      </c>
+      <c r="D10" s="19">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C11" s="19">
+        <v>45</v>
+      </c>
+      <c r="D11" s="19">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="C17" s="1">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C22" s="1">
+        <v>33</v>
+      </c>
+      <c r="D22" s="1">
+        <v>48</v>
+      </c>
+      <c r="E22" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1">
+        <v>35</v>
+      </c>
+      <c r="E23" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1">
+        <v>38</v>
+      </c>
+      <c r="E24" s="1">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4495,7 +4932,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17765,7 +18202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="A10:C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18186,8 +18625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>